<commit_message>
result excel api working done
</commit_message>
<xml_diff>
--- a/public/uploads/Results_Template.xlsx
+++ b/public/uploads/Results_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanyammahajan/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sms\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6D3716-BA6C-164D-A83B-F39BC1013058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A926B8E0-A8D1-452A-88C4-DCDCA33CD8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,46 +22,46 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
-    <t>StudentID</t>
-  </si>
-  <si>
-    <t>SubjectCode</t>
-  </si>
-  <si>
-    <t>SessionalExam</t>
-  </si>
-  <si>
-    <t>EndTerm</t>
-  </si>
-  <si>
-    <t>OverallMark</t>
-  </si>
-  <si>
     <t>Grade</t>
   </si>
   <si>
-    <t>2023-104</t>
-  </si>
-  <si>
-    <t>2023-15</t>
-  </si>
-  <si>
-    <t>2023-115</t>
-  </si>
-  <si>
     <t>DAM-101</t>
   </si>
   <si>
-    <t>DAM-102</t>
-  </si>
-  <si>
-    <t>DAM-103</t>
-  </si>
-  <si>
     <t>C+</t>
   </si>
   <si>
     <t>B+</t>
+  </si>
+  <si>
+    <t>Roll No</t>
+  </si>
+  <si>
+    <t>Subject Code</t>
+  </si>
+  <si>
+    <t>Sessional Exam</t>
+  </si>
+  <si>
+    <t>End Term</t>
+  </si>
+  <si>
+    <t>Overall Mark</t>
+  </si>
+  <si>
+    <t>2023-133</t>
+  </si>
+  <si>
+    <t>2023-156</t>
+  </si>
+  <si>
+    <t>2023-122</t>
+  </si>
+  <si>
+    <t>DAP-102</t>
+  </si>
+  <si>
+    <t>DAC-103</t>
   </si>
 </sst>
 </file>
@@ -438,37 +438,45 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -480,15 +488,15 @@
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>18</v>
@@ -500,15 +508,15 @@
         <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>22</v>
@@ -520,7 +528,7 @@
         <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
result verification handled smoothly
</commit_message>
<xml_diff>
--- a/public/uploads/Results_Template.xlsx
+++ b/public/uploads/Results_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sms\public\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanyammahajan/Documents/GitHub/ISTC-SMS-New/public/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E2BD09-5686-450A-83B1-2665D85D2932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F2813E-E6A3-7045-B670-EC1B7AD1A5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>DAM-101</t>
-  </si>
-  <si>
     <t>C+</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>2023-122</t>
+  </si>
+  <si>
+    <t>DME-105</t>
   </si>
 </sst>
 </file>
@@ -432,45 +432,45 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -482,15 +482,15 @@
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>18</v>
@@ -502,15 +502,15 @@
         <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
       </c>
       <c r="C4">
         <v>22</v>
@@ -522,7 +522,7 @@
         <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>